<commit_message>
BCRA-31 - Family History Questions
Change-Id: Idee8a7b4068101be2cc1aa6ff6d1cf0ffee675ff
</commit_message>
<xml_diff>
--- a/data/questionnaires/version1/question_section.xlsx
+++ b/data/questionnaires/version1/question_section.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>PERSONAL_HISTORY</t>
   </si>
@@ -70,6 +70,39 @@
   </si>
   <si>
     <t>FAMILY_OVARIAN</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>consent</t>
+  </si>
+  <si>
+    <t>family</t>
+  </si>
+  <si>
+    <t>breast</t>
+  </si>
+  <si>
+    <t>ovarian</t>
+  </si>
+  <si>
+    <t>grandmother</t>
+  </si>
+  <si>
+    <t>aunt</t>
+  </si>
+  <si>
+    <t>niece</t>
+  </si>
+  <si>
+    <t>halfsister</t>
+  </si>
+  <si>
+    <t>history</t>
   </si>
 </sst>
 </file>
@@ -408,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +456,7 @@
     <col min="8" max="8" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -442,8 +475,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -462,8 +501,14 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -482,8 +527,14 @@
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -502,8 +553,14 @@
       <c r="F4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -522,8 +579,14 @@
       <c r="F5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -542,8 +605,14 @@
       <c r="F6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -562,8 +631,14 @@
       <c r="F7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -582,8 +657,14 @@
       <c r="F8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -602,8 +683,14 @@
       <c r="F9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -621,6 +708,12 @@
       </c>
       <c r="F10">
         <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>